<commit_message>
feature udistrital/sga_documentacion#121 Finalización reporte
Se realizan las consultas para completar el reporte
</commit_message>
<xml_diff>
--- a/static/templates/PruebaExcel.xlsx
+++ b/static/templates/PruebaExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\moreraz\go\src\github.com\udistrital\sga_admisiones_mid\static\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BFAAE2-C94C-409A-8CA1-277A0922FABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17FD77A-B774-4399-B210-F079AC7C0B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4F02024F-C3A6-4CB6-B2A9-76C0CAFA61C4}"/>
   </bookViews>
@@ -161,46 +161,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -574,7 +571,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:G5"/>
+      <selection activeCell="B4" sqref="B4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,51 +584,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="4"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="4"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="10"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
       <c r="G4" s="11"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="13"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -646,13 +643,13 @@
       <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>